<commit_message>
first version that should work on server
</commit_message>
<xml_diff>
--- a/report_folder/report_0_gruppe.xlsx
+++ b/report_folder/report_0_gruppe.xlsx
@@ -4296,7 +4296,7 @@
         </is>
       </c>
       <c r="C17" s="13" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F17" s="14" t="inlineStr">
         <is>
@@ -4304,7 +4304,7 @@
         </is>
       </c>
       <c r="G17" s="35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -4315,7 +4315,7 @@
       </c>
       <c r="C18" s="13" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D18" s="14" t="inlineStr">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="D19" s="26" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F19" s="14" t="inlineStr">
@@ -4349,7 +4349,7 @@
         </is>
       </c>
       <c r="G19" s="35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -4370,7 +4370,7 @@
       </c>
       <c r="D20" s="25" t="inlineStr">
         <is>
-          <t>40.0% der Karten</t>
+          <t>37.5% der Karten</t>
         </is>
       </c>
     </row>
@@ -4379,7 +4379,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="36" t="inlineStr">
         <is>
@@ -4421,7 +4421,7 @@
         </is>
       </c>
       <c r="C27" s="14" t="n">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="D27" s="14" t="n"/>
       <c r="E27" s="35" t="n"/>
@@ -4436,7 +4436,7 @@
         </is>
       </c>
       <c r="C28" s="14" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D28" s="14" t="n"/>
       <c r="E28" s="35" t="n"/>
@@ -4447,11 +4447,11 @@
       <c r="A29" s="14" t="n"/>
       <c r="B29" s="14" t="inlineStr">
         <is>
-          <t>Gruppentreffen 08.06.2020 💩</t>
+          <t>Gruppentreffen 29.06.2020 💩</t>
         </is>
       </c>
       <c r="C29" s="14" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D29" s="14" t="n"/>
       <c r="E29" s="35" t="n"/>
@@ -4462,11 +4462,11 @@
       <c r="A30" s="14" t="n"/>
       <c r="B30" s="14" t="inlineStr">
         <is>
-          <t>Gruppentreffen 💩</t>
+          <t>Gruppentreffen 06.07.2020</t>
         </is>
       </c>
       <c r="C30" s="14" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D30" s="14" t="n"/>
       <c r="E30" s="35" t="n"/>
@@ -4477,11 +4477,11 @@
       <c r="A31" s="14" t="n"/>
       <c r="B31" s="14" t="inlineStr">
         <is>
-          <t>Gruppentreffen 29.06.2020 💩</t>
+          <t>Gruppentreffen 13.07.2020</t>
         </is>
       </c>
       <c r="C31" s="14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D31" s="14" t="n"/>
       <c r="E31" s="35" t="n"/>
@@ -4536,7 +4536,7 @@
         </is>
       </c>
       <c r="C35" s="14" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
@@ -4551,7 +4551,7 @@
         </is>
       </c>
       <c r="C36" s="14" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
@@ -4566,7 +4566,7 @@
         </is>
       </c>
       <c r="C37" s="14" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
@@ -4581,7 +4581,7 @@
         </is>
       </c>
       <c r="C38" s="14" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
@@ -4596,7 +4596,7 @@
         </is>
       </c>
       <c r="C39" s="14" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -4604,7 +4604,7 @@
         </is>
       </c>
       <c r="F39" s="14" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
@@ -4614,7 +4614,7 @@
         </is>
       </c>
       <c r="F40" s="14" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41">
@@ -4624,7 +4624,7 @@
         </is>
       </c>
       <c r="F41" s="14" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42">
@@ -4634,7 +4634,7 @@
         </is>
       </c>
       <c r="F42" s="14" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
@@ -4644,7 +4644,7 @@
         </is>
       </c>
       <c r="F43" s="14" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row customHeight="1" ht="20" r="46">
@@ -4673,7 +4673,7 @@
         </is>
       </c>
       <c r="C48" s="14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -4688,7 +4688,7 @@
         </is>
       </c>
       <c r="C49" s="14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -4703,12 +4703,15 @@
         </is>
       </c>
       <c r="C50" s="14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E50" s="14" t="inlineStr">
         <is>
-          <t>Aktivste Helfer</t>
-        </is>
+          <t>Maria Lütticke</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -4723,10 +4726,15 @@
         </is>
       </c>
       <c r="C51" s="14" t="n">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Peter Augustin</t>
+        </is>
       </c>
       <c r="F51" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -4741,20 +4749,35 @@
         </is>
       </c>
       <c r="C52" s="14" t="n">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Noah Brechmann</t>
+        </is>
       </c>
       <c r="F52" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Christoph Netsch</t>
+        </is>
+      </c>
       <c r="F53" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Jacob Escherich</t>
+        </is>
+      </c>
       <c r="F54" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -4784,7 +4807,7 @@
         </is>
       </c>
       <c r="G60" s="35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61">
@@ -4863,10 +4886,15 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Christoph Netsch</t>
+        </is>
       </c>
       <c r="G70" s="35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -4876,10 +4904,15 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Eric Pomp</t>
+        </is>
       </c>
       <c r="G71" s="35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
@@ -4892,8 +4925,13 @@
         <f>B70-B71-B73</f>
         <v/>
       </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Jacob Escherich</t>
+        </is>
+      </c>
       <c r="G72" s="35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -4903,15 +4941,25 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Maria Lütticke</t>
+        </is>
       </c>
       <c r="G73" s="35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Marie-Sophie Braun</t>
+        </is>
+      </c>
       <c r="G74" s="35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">

</xml_diff>